<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig@76aa80cfe7784591589aa19e57658a46b3f451fb 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-ncpi.xlsx
+++ b/CodeSystem-ncpi.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-09-13T16:54:38+00:00</t>
+    <t>2022-10-11T14:45:04+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>Study Cohort</t>
+  </si>
+  <si>
+    <t>ConsentGroup</t>
+  </si>
+  <si>
+    <t>Study Consent Group</t>
   </si>
   <si>
     <t>Summary</t>
@@ -507,7 +513,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -671,6 +677,18 @@
       </c>
       <c r="D13" s="2"/>
     </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>